<commit_message>
Add info to file information
</commit_message>
<xml_diff>
--- a/Information.xlsx
+++ b/Information.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="23070" windowHeight="9015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="23076" windowHeight="9012" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Протокол" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Убрать зависимоть FILE от OBJECT</t>
   </si>
@@ -110,6 +110,59 @@
   </si>
   <si>
     <t>Завершено</t>
+  </si>
+  <si>
+    <t>Установка</t>
+  </si>
+  <si>
+    <t>Настройка</t>
+  </si>
+  <si>
+    <t>Верхнее меню -&gt; Git -&gt; Параметры -&gt; Система управления версиями -&gt; Параметры Git-репозитория -&gt; Удалённые -&gt; Добавить : GitHub https://github.com/tabakov-ma/GENA.git 
+(при подключении user: tabakov-ma, pass: maT_1319023008 )</t>
+  </si>
+  <si>
+    <t>Клиент 1. Создание изменений в проекте (изменеие, добавление или удаление)</t>
+  </si>
+  <si>
+    <t>В окне вывода проконтролировать выполнение</t>
+  </si>
+  <si>
+    <t>Клиент 1. Верхнее меню -&gt; Git -&gt; Изменения Git: ввести сообщение об изменениях, 
+нажать кнопку зафиксировать всё и нажать кнопку синхронизировать</t>
+  </si>
+  <si>
+    <t>Клиент 2. п.1</t>
+  </si>
+  <si>
+    <t>Клиент 2. п.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Клиент 2. Нижнее окно -&gt; Список ошибок -&gt; Перечень конфликтов слияния: 
+перейти в редактор кода в место конфликта </t>
+  </si>
+  <si>
+    <t>Клиент 2. В верхней части редактора кода есть сообщение: "Файл содержит конфлик слияния",
+нажать рядом на "Открыть редактор слияния"</t>
+  </si>
+  <si>
+    <t>Клиент 2. В редакторе слияний применить входящие и/или 
+применить текущие и нажать применить слияние</t>
+  </si>
+  <si>
+    <t>Клиент 2. п.2 (сообщение аналогичное п.4)</t>
+  </si>
+  <si>
+    <t>Использование (пример)</t>
+  </si>
+  <si>
+    <t>Клиент 1. Без создания изменений в проекте</t>
+  </si>
+  <si>
+    <t>Клиент 1. Верхнее меню -&gt; Git -&gt; Изменения Git: нажать кнопку синхронизировать</t>
+  </si>
+  <si>
+    <t>При это в проет должны зайти все изменения из хранилище данных GitHub</t>
   </si>
 </sst>
 </file>
@@ -119,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +194,39 @@
       <name val="SimSun-ExtB"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -183,6 +262,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -480,20 +568,20 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="28" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="101" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -522,7 +610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="86.25">
+    <row r="2" spans="1:8" ht="64.8">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -574,7 +662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34.5">
+    <row r="4" spans="1:8">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -624,7 +712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34.5">
+    <row r="6" spans="1:8" ht="32.4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1074,32 +1162,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="10"/>
+    <col min="2" max="2" width="85.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="43.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="10" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8">
+      <c r="A10" s="10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="10">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8">
+      <c r="A13" s="10">
+        <v>5</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8">
+      <c r="A15" s="10">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="10">
+        <v>8</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="10">
+        <v>9</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10">
+        <v>10</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1108,31 +1312,31 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18">
+    <row r="1" spans="1:1" ht="17.399999999999999">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Добавил через NuGet Microsoft.SqlServer.Compact
</commit_message>
<xml_diff>
--- a/Information.xlsx
+++ b/Information.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="23076" windowHeight="9012" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="23076" windowHeight="9012"/>
   </bookViews>
   <sheets>
     <sheet name="Протокол" sheetId="1" r:id="rId1"/>
     <sheet name="GitHub" sheetId="2" r:id="rId2"/>
-    <sheet name="Service" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Service" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="DARBL">Service!$A$2:$A$4</definedName>
@@ -24,16 +24,9 @@
     <t>Убрать зависимоть FILE от OBJECT</t>
   </si>
   <si>
-    <t>А. Необходимо дороботать зависимости постоянно активные, и файлы специфичные для объектов будут связываться сдесь, пометка о специфичности файлов будет указываться в таблице ListFILE
-Б. В заголовок таблицы добавлять только главгые объекты</t>
-  </si>
-  <si>
     <t>Relation_File_Obj</t>
   </si>
   <si>
-    <t>Конструктор таблиц</t>
-  </si>
-  <si>
     <t xml:space="preserve">Авторазмер ширины окна </t>
   </si>
   <si>
@@ -116,10 +109,6 @@
   </si>
   <si>
     <t>Настройка</t>
-  </si>
-  <si>
-    <t>Верхнее меню -&gt; Git -&gt; Параметры -&gt; Система управления версиями -&gt; Параметры Git-репозитория -&gt; Удалённые -&gt; Добавить : GitHub https://github.com/tabakov-ma/GENA.git 
-(при подключении user: tabakov-ma, pass: maT_1319023008 )</t>
   </si>
   <si>
     <t>Клиент 1. Создание изменений в проекте (изменеие, добавление или удаление)</t>
@@ -163,6 +152,17 @@
   </si>
   <si>
     <t>При это в проет должны зайти все изменения из хранилище данных GitHub</t>
+  </si>
+  <si>
+    <t>Верхнее меню -&gt; Git -&gt; Параметры -&gt; Система управления версиями -&gt; Параметры Git-репозитория -&gt; Удалённые -&gt; Добавить : GitHub https://github.com/tabakov-ma/GENA.git 
+(при подключении Администратор user: tabakov-ma, pass: maT_1319023008, подключаться под своей учёткой )</t>
+  </si>
+  <si>
+    <t>А. Необходимо дороботать зависимости постоянно активные, и файлы специфичные для объектов будут связываться сдесь, пометка о специфичности файлов будет указываться в таблице ListFILE
+Б. В заголовок таблицы добавлять только главные объекты</t>
+  </si>
+  <si>
+    <t>Конструктор таблиц, главная форма проводника</t>
   </si>
 </sst>
 </file>
@@ -567,18 +567,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="66.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="101" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="3"/>
@@ -586,31 +586,31 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="64.8">
+    </row>
+    <row r="2" spans="1:8" ht="121.2" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -618,25 +618,25 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="48.6">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -644,22 +644,22 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -670,25 +670,25 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24.6" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -696,20 +696,20 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="32.4">
@@ -720,22 +720,22 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -746,20 +746,20 @@
         <v>44741.416666666664</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1178,12 +1178,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1191,25 +1191,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6">
       <c r="A6" s="10">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8">
@@ -1225,10 +1225,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1236,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1244,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8">
@@ -1252,7 +1252,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8">
@@ -1260,7 +1260,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8">
@@ -1268,7 +1268,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1276,10 +1276,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1287,7 +1287,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1295,10 +1295,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1322,22 +1322,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="17.399999999999999">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>